<commit_message>
Up to excercise 10
</commit_message>
<xml_diff>
--- a/Sprint2Tema1Ejercicios.xlsx
+++ b/Sprint2Tema1Ejercicios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Barajas\Desktop\02 PHP FULL STACK\Sprint 2\Sprint2Tema1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{7E9FB2E0-F9FC-490A-937A-5891AE916D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{F766FEA1-E574-4661-9109-7DCF2EAA6EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-700" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
@@ -65,12 +65,6 @@
     <t>Lista los nombres y precios de todos los productos de la tabla "producto", truncando el valor del precio para mostrarlo sin ninguna cifra decimal.</t>
   </si>
   <si>
-    <t>Lista el código de los fabricantes que tienen productos en la mesa "producto".</t>
-  </si>
-  <si>
-    <t>Lista el código de los fabricantes que tienen productos en la mesa "producto", eliminando los códigos que aparecen repetidos.</t>
-  </si>
-  <si>
     <t>Lista los nombres de los fabricantes ordenados de forma ascendente.</t>
   </si>
   <si>
@@ -165,6 +159,12 @@
   </si>
   <si>
     <t>Lista los nombres y precios de todos los productos de la tabla "producto", redondeando el valor del precio.</t>
+  </si>
+  <si>
+    <t>Lista el código de los fabricantes que tienen productos en la tabla "producto".</t>
+  </si>
+  <si>
+    <t>Lista el código de los fabricantes que tienen productos en la tabla "producto", eliminando los códigos que aparecen repetidos.</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,10 +581,10 @@
   <sheetData>
     <row r="1" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -664,7 +664,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -682,7 +682,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -691,7 +691,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -700,7 +700,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -709,7 +709,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="31" x14ac:dyDescent="0.35">
@@ -718,7 +718,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -727,7 +727,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -736,7 +736,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="31" x14ac:dyDescent="0.35">
@@ -745,7 +745,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="31" x14ac:dyDescent="0.35">
@@ -754,7 +754,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -763,7 +763,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -772,7 +772,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="31" x14ac:dyDescent="0.35">
@@ -781,7 +781,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="31" x14ac:dyDescent="0.35">
@@ -790,7 +790,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -799,7 +799,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -808,7 +808,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -817,7 +817,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -826,7 +826,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -835,7 +835,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -844,7 +844,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -853,7 +853,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -862,7 +862,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="31" x14ac:dyDescent="0.35">
@@ -871,7 +871,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -880,7 +880,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="31" x14ac:dyDescent="0.35">
@@ -889,7 +889,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -898,7 +898,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -907,7 +907,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -916,7 +916,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -925,7 +925,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -934,7 +934,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -943,7 +943,7 @@
         <v>40</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -952,7 +952,7 @@
         <v>41</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done until Excercise 23
</commit_message>
<xml_diff>
--- a/Sprint2Tema1Ejercicios.xlsx
+++ b/Sprint2Tema1Ejercicios.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Barajas\Desktop\02 PHP FULL STACK\Sprint 2\Sprint2Tema1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{F766FEA1-E574-4661-9109-7DCF2EAA6EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A45443-94AC-48AA-8570-BCF435122360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-700" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-19310" yWindow="-700" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ejercicios" sheetId="1" r:id="rId1"/>
@@ -74,12 +74,6 @@
     <t>Lista los nombres de los productos ordenados, en primer lugar, por el nombre de forma ascendente y, en segundo lugar, por el precio de forma descendente.</t>
   </si>
   <si>
-    <t>Devuelve una lista con las 5 primeras filas de la mesa "fabricante".</t>
-  </si>
-  <si>
-    <t>Devuelve una lista con 2 filas a partir de la cuarta fila de la mesa "fabricante". La cuarta fila también debe incluirse en la respuesta.</t>
-  </si>
-  <si>
     <t>Lista el nombre y precio del producto más barato. (Utiliza solo las cláusulas ORDER BY y LIMIT). NOTA: Aquí no podrías usar MIN(precio), necesitarías GROUP BY</t>
   </si>
   <si>
@@ -165,12 +159,18 @@
   </si>
   <si>
     <t>Lista el código de los fabricantes que tienen productos en la tabla "producto", eliminando los códigos que aparecen repetidos.</t>
+  </si>
+  <si>
+    <t>Devuelve una lista con las 5 primeras filas de la tabla "fabricante".</t>
+  </si>
+  <si>
+    <t>Devuelve una lista con 2 filas a partir de la cuarta fila de la tabla "fabricante". La cuarta fila también debe incluirse en la respuesta.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -565,26 +565,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.6328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.90625" style="2" customWidth="1"/>
     <col min="3" max="3" width="141.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -664,7 +664,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -677,120 +677,120 @@
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="3">
+      <c r="B12" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+      <c r="B16" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B17" s="6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
+    <row r="18" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="6">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+      <c r="B19" s="6">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="20" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+      <c r="B20" s="6">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="21" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B21" s="6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B16" s="3">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B17" s="3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B18" s="3">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="22" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B22" s="6">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B19" s="3">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="23" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+      <c r="B23" s="6">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B20" s="3">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="24" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+      <c r="B24" s="6">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B21" s="3">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B22" s="3">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B23" s="3">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B24" s="3">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -799,7 +799,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -808,7 +808,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -817,7 +817,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -826,7 +826,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -835,7 +835,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -844,7 +844,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -853,7 +853,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -862,7 +862,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="31" x14ac:dyDescent="0.35">
@@ -871,7 +871,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -880,7 +880,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="31" x14ac:dyDescent="0.35">
@@ -889,7 +889,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -898,7 +898,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -907,7 +907,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -916,7 +916,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -925,7 +925,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -934,7 +934,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -943,7 +943,7 @@
         <v>40</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -952,7 +952,7 @@
         <v>41</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excercise usig Universidad DB done until excercise 9
</commit_message>
<xml_diff>
--- a/Sprint2Tema1Ejercicios.xlsx
+++ b/Sprint2Tema1Ejercicios.xlsx
@@ -8,14 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Barajas\Desktop\02 PHP FULL STACK\Sprint 2\Sprint2Tema1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F6F87A-FC3C-4F57-A6C9-4BD85261FC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3D1275-F109-460F-86A7-38FAE237A6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="564" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ejercicios" sheetId="1" r:id="rId1"/>
+    <sheet name="Tienda" sheetId="1" r:id="rId1"/>
     <sheet name="producto" sheetId="2" r:id="rId2"/>
     <sheet name="fabricante" sheetId="3" r:id="rId3"/>
+    <sheet name="Universidad" sheetId="4" r:id="rId4"/>
+    <sheet name="alumno_se_matricula_asignatura" sheetId="5" r:id="rId5"/>
+    <sheet name="asignatura" sheetId="6" r:id="rId6"/>
+    <sheet name="curso_escolar" sheetId="7" r:id="rId7"/>
+    <sheet name="departamento" sheetId="8" r:id="rId8"/>
+    <sheet name="grado" sheetId="9" r:id="rId9"/>
+    <sheet name="persona" sheetId="10" r:id="rId10"/>
+    <sheet name="profesor" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">producto!$A$1:$D$12</definedName>
@@ -41,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
   <si>
     <t>Lista los nombres y precios de todos los productos de la tabla "producto".</t>
   </si>
@@ -254,13 +262,99 @@
   </si>
   <si>
     <t>Lista el nombre de todos los productos que hay en la tabla "producto".</t>
+  </si>
+  <si>
+    <t>1. Retorna un llistat amb el primer cognom, segon cognom i el nom de tots els/les alumnes. El llistat haurà d'estar ordenat alfabèticament de menor a major pel primer cognom, segon cognom i nom.</t>
+  </si>
+  <si>
+    <t>3. Retorna el llistat dels/les alumnes que van néixer en 1999.</t>
+  </si>
+  <si>
+    <t>4. Retorna el llistat de professors/es que no han donat d'alta el seu número de telèfon en la base de dades i a més el seu NIF acaba en K.</t>
+  </si>
+  <si>
+    <t>5. Retorna el llistat de les assignatures que s'imparteixen en el primer quadrimestre, en el tercer curs del grau que té l'identificador 7.</t>
+  </si>
+  <si>
+    <t>9. Retorna un llistat amb tots els/les alumnes que s'han matriculat en alguna assignatura durant el curs escolar 2018/2019.</t>
+  </si>
+  <si>
+    <t>Resol les 6 següents consultes utilitzant les clàusules LEFT JOIN i RIGHT JOIN.</t>
+  </si>
+  <si>
+    <t>1.  Retorna un llistat amb els noms de tots els professors/es i els departaments que tenen vinculats/des. El llistat també ha de mostrar aquells professors/es que no tenen cap departament associat. El llistat ha de retornar quatre columnes, nom del departament, primer cognom, segon cognom i nom del professor/a. El resultat estarà ordenat alfabèticament de menor a major pel nom del departament, cognoms i el nom.</t>
+  </si>
+  <si>
+    <t>2. Retorna un llistat amb els professors/es que no estan associats a un departament.</t>
+  </si>
+  <si>
+    <t>3. Retorna un llistat amb els departaments que no tenen professors/es associats.</t>
+  </si>
+  <si>
+    <t>4. Retorna un llistat amb els professors/es que no imparteixen cap assignatura.</t>
+  </si>
+  <si>
+    <t>5. Retorna un llistat amb les assignatures que no tenen un professor/a assignat.</t>
+  </si>
+  <si>
+    <t>6. Retorna un llistat amb tots els departaments que no han impartit assignatures en cap curs escolar.</t>
+  </si>
+  <si>
+    <t>Consultes resum:</t>
+  </si>
+  <si>
+    <t>1. Retorna el nombre total d'alumnes que hi ha.</t>
+  </si>
+  <si>
+    <t>2. Calcula quants/es alumnes van néixer en 1999.</t>
+  </si>
+  <si>
+    <t>3. Calcula quants/es professors/es hi ha en cada departament. El resultat només ha de mostrar dues columnes, una amb el nom del departament i una altra amb el nombre de professors/es que hi ha en aquest departament. El resultat només ha d'incloure els departaments que tenen professors/es associats i haurà d'estar ordenat de major a menor pel nombre de professors/es.</t>
+  </si>
+  <si>
+    <t>4. Retorna un llistat amb tots els departaments i el nombre de professors/es que hi ha en cadascun d'ells. Té en compte que poden existir departaments que no tenen professors/es associats/des. Aquests departaments també han d'aparèixer en el llistat.</t>
+  </si>
+  <si>
+    <t>5. Retorna un llistat amb el nom de tots els graus existents en la base de dades i el nombre d'assignatures que té cadascun. Té en compte que poden existir graus que no tenen assignatures associades. Aquests graus també han d'aparèixer en el llistat. El resultat haurà d'estar ordenat de major a menor pel nombre d'assignatures.</t>
+  </si>
+  <si>
+    <t>6. Retorna un llistat amb el nom de tots els graus existents en la base de dades i el nombre d'assignatures que té cadascun, dels graus que tinguin més de 40 assignatures associades.</t>
+  </si>
+  <si>
+    <t>7. Retorna un llistat que mostri el nom dels graus i la suma del nombre total de crèdits que hi ha per a cada tipus d'assignatura. El resultat ha de tenir tres columnes: nom del grau, tipus d'assignatura i la suma dels crèdits de totes les assignatures que hi ha d'aquest tipus.</t>
+  </si>
+  <si>
+    <t>8. Retorna un llistat que mostri quants/es alumnes s'han matriculat d'alguna assignatura en cadascun dels cursos escolars. El resultat haurà de mostrar dues columnes, una columna amb l'any d'inici del curs escolar i una altra amb el nombre d'alumnes matriculats/des.</t>
+  </si>
+  <si>
+    <t>9. Retorna un llistat amb el nombre d'assignatures que imparteix cada professor/a. El llistat ha de tenir en compte aquells professors/es que no imparteixen cap assignatura. El resultat mostrarà cinc columnes: id, nom, primer cognom, segon cognom i nombre d'assignatures. El resultat estarà ordenat de major a menor pel nombre d'assignatures.</t>
+  </si>
+  <si>
+    <t>10. Retorna totes les dades de l'alumne més jove.</t>
+  </si>
+  <si>
+    <t>11. Retorna un llistat amb els professors/es que tenen un departament associat i que no imparteixen cap assignatura.</t>
+  </si>
+  <si>
+    <t>Halla el nombre y los dos apellidos de los alumnos que no han dado de alta su número de teléfono en la base de datos.</t>
+  </si>
+  <si>
+    <t>Retorna un llistat dels professors/es juntament amb el nom del departament al qual estan vinculats/des. 
+El llistat ha de retornar quatre columnes, primer cognom, segon cognom, nom i nom del departament. 
+El resultat estarà ordenat alfabèticament de menor a major pels cognoms i el nom.</t>
+  </si>
+  <si>
+    <t>Retorna un llistat amb el nom de les assignatures, any d'inici i any de fi del curs escolar de l'alumne/a amb NIF 26902806M.</t>
+  </si>
+  <si>
+    <t>Retorna un llistat amb el nom de tots els departaments que tenen professors/es que imparteixen alguna assignatura en el Grau en Enginyeria Informàtica (Pla 2015).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +380,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF202124"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -338,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -370,6 +472,24 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -685,398 +805,424 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C42"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42:C42"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="6.90625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="141.36328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.90625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="141.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <f t="shared" ref="A4:A42" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B15" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="4">
-        <f>B2+1</f>
-        <v>2</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="4">
-        <f t="shared" ref="B4:B42" si="0">B3+1</f>
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B6" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="4">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="4">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="4">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B16" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="4">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="4">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="4">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="4">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="4">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="4">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A33" s="4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="4">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A35" s="4">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="4">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="10">
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="4">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B38" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="8">
+        <f>A38+1</f>
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="4">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="B39" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="8">
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B14" s="4">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="4">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B16" s="4">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B17" s="4">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="B40" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="10">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B18" s="4">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B41" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="10">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B19" s="4">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B20" s="4">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B21" s="4">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B22" s="4">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B23" s="4">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B24" s="4">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B25" s="4">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B26" s="4">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B27" s="4">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B28" s="4">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B29" s="4">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B30" s="4">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B31" s="4">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B32" s="4">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B33" s="4">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B34" s="4">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="B35" s="4">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B36" s="4">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B37" s="4">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B38" s="10">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B39" s="8">
-        <f>B38+1</f>
-        <v>38</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B40" s="8">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B41" s="10">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B42" s="10">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="C42" s="11" t="s">
+      <c r="B42" s="11" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5DD659F-EA35-467C-B419-FF376CE605B4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C19AC5-F112-4205-A84D-1D30622B7634}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1370,4 +1516,335 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F9DC3-8699-4E47-BF29-61940CBB7A2D}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.1796875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="104.7265625" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+      <c r="A3" s="17">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="17">
+        <f t="shared" ref="A4:A10" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+      <c r="A5" s="17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+      <c r="A6" s="17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+      <c r="A8" s="17">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+      <c r="A9" s="17">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+      <c r="A10" s="15">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="62" x14ac:dyDescent="0.35">
+      <c r="A12" s="15">
+        <v>1</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="15">
+        <f>A12+1</f>
+        <v>2</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="15">
+        <f t="shared" ref="A14:A17" si="1">A13+1</f>
+        <v>3</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="15">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="15">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="15">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="15">
+        <v>1</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="15">
+        <f>A19+1</f>
+        <v>2</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+      <c r="A21" s="15">
+        <f t="shared" ref="A21:A29" si="2">A20+1</f>
+        <v>3</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A24" s="15">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="15">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="15">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+      <c r="A27" s="15">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="15">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A29" s="15">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC2CCD8-C735-4335-9847-11758075F4AE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B8E14E-1DEA-4122-9E07-CDFCFC5B0CF7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27302FC0-D1D1-4197-9409-D0DDD97304F2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D068D9-3CAA-456E-AF7B-1581F08CA8BC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25C70BF-5A5B-49AF-9C74-9219450E7959}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Universidad excercises done until 6
</commit_message>
<xml_diff>
--- a/Sprint2Tema1Ejercicios.xlsx
+++ b/Sprint2Tema1Ejercicios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Barajas\Desktop\02 PHP FULL STACK\Sprint 2\Sprint2Tema1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3D1275-F109-460F-86A7-38FAE237A6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD5404C-4815-49D0-BF02-C967619AA520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="564" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="466" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tienda" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,9 @@
     <sheet name="profesor" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">persona!$A$1:$K$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">producto!$A$1:$D$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">profesor!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="231">
   <si>
     <t>Lista los nombres y precios de todos los productos de la tabla "producto".</t>
   </si>
@@ -282,18 +284,9 @@
     <t>Resol les 6 següents consultes utilitzant les clàusules LEFT JOIN i RIGHT JOIN.</t>
   </si>
   <si>
-    <t>1.  Retorna un llistat amb els noms de tots els professors/es i els departaments que tenen vinculats/des. El llistat també ha de mostrar aquells professors/es que no tenen cap departament associat. El llistat ha de retornar quatre columnes, nom del departament, primer cognom, segon cognom i nom del professor/a. El resultat estarà ordenat alfabèticament de menor a major pel nom del departament, cognoms i el nom.</t>
-  </si>
-  <si>
-    <t>2. Retorna un llistat amb els professors/es que no estan associats a un departament.</t>
-  </si>
-  <si>
     <t>3. Retorna un llistat amb els departaments que no tenen professors/es associats.</t>
   </si>
   <si>
-    <t>4. Retorna un llistat amb els professors/es que no imparteixen cap assignatura.</t>
-  </si>
-  <si>
     <t>5. Retorna un llistat amb les assignatures que no tenen un professor/a assignat.</t>
   </si>
   <si>
@@ -307,18 +300,6 @@
   </si>
   <si>
     <t>2. Calcula quants/es alumnes van néixer en 1999.</t>
-  </si>
-  <si>
-    <t>3. Calcula quants/es professors/es hi ha en cada departament. El resultat només ha de mostrar dues columnes, una amb el nom del departament i una altra amb el nombre de professors/es que hi ha en aquest departament. El resultat només ha d'incloure els departaments que tenen professors/es associats i haurà d'estar ordenat de major a menor pel nombre de professors/es.</t>
-  </si>
-  <si>
-    <t>4. Retorna un llistat amb tots els departaments i el nombre de professors/es que hi ha en cadascun d'ells. Té en compte que poden existir departaments que no tenen professors/es associats/des. Aquests departaments també han d'aparèixer en el llistat.</t>
-  </si>
-  <si>
-    <t>5. Retorna un llistat amb el nom de tots els graus existents en la base de dades i el nombre d'assignatures que té cadascun. Té en compte que poden existir graus que no tenen assignatures associades. Aquests graus també han d'aparèixer en el llistat. El resultat haurà d'estar ordenat de major a menor pel nombre d'assignatures.</t>
-  </si>
-  <si>
-    <t>6. Retorna un llistat amb el nom de tots els graus existents en la base de dades i el nombre d'assignatures que té cadascun, dels graus que tinguin més de 40 assignatures associades.</t>
   </si>
   <si>
     <t>7. Retorna un llistat que mostri el nom dels graus i la suma del nombre total de crèdits que hi ha per a cada tipus d'assignatura. El resultat ha de tenir tres columnes: nom del grau, tipus d'assignatura i la suma dels crèdits de totes les assignatures que hi ha d'aquest tipus.</t>
@@ -348,6 +329,433 @@
   </si>
   <si>
     <t>Retorna un llistat amb el nom de tots els departaments que tenen professors/es que imparteixen alguna assignatura en el Grau en Enginyeria Informàtica (Pla 2015).</t>
+  </si>
+  <si>
+    <t>Retorna un listado con los nombres de todos los profesores/as y los departamentos que tienen vinculados/as. 
+El listado también debe mostrar aquellos profesores/as que no tienen ningún departamento asociado. 
+El listado debe devolver cuatro columnas, nombre del departamento, primer apellido, segundo apellido y nombre del profesor/a. 
+El resultado estará ordenado alfabéticamente de menor a mayor por el nombre del departamento, apellidos y nombre.</t>
+  </si>
+  <si>
+    <t>Retorna un llistat amb els professors/es que no estan associats a un departament.</t>
+  </si>
+  <si>
+    <t>26902806M</t>
+  </si>
+  <si>
+    <t>Salvador</t>
+  </si>
+  <si>
+    <t>Sánchez</t>
+  </si>
+  <si>
+    <t>Pérez</t>
+  </si>
+  <si>
+    <t>Almería</t>
+  </si>
+  <si>
+    <t>C/ Real del barrio alto</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>alumno</t>
+  </si>
+  <si>
+    <t>89542419S</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Saez</t>
+  </si>
+  <si>
+    <t>Vega</t>
+  </si>
+  <si>
+    <t>C/ Mercurio</t>
+  </si>
+  <si>
+    <t>11105554G</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>Ramirez</t>
+  </si>
+  <si>
+    <t>Gea</t>
+  </si>
+  <si>
+    <t>C/ Marte</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>profesor</t>
+  </si>
+  <si>
+    <t>17105885A</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Heller</t>
+  </si>
+  <si>
+    <t>Pagac</t>
+  </si>
+  <si>
+    <t>C/ Estrella fugaz</t>
+  </si>
+  <si>
+    <t>38223286T</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Schmidt</t>
+  </si>
+  <si>
+    <t>Fisher</t>
+  </si>
+  <si>
+    <t>C/ Venus</t>
+  </si>
+  <si>
+    <t>04233869Y</t>
+  </si>
+  <si>
+    <t>José</t>
+  </si>
+  <si>
+    <t>Koss</t>
+  </si>
+  <si>
+    <t>Bayer</t>
+  </si>
+  <si>
+    <t>C/ Júpiter</t>
+  </si>
+  <si>
+    <t>97258166K</t>
+  </si>
+  <si>
+    <t>Ismael</t>
+  </si>
+  <si>
+    <t>Strosin</t>
+  </si>
+  <si>
+    <t>Turcotte</t>
+  </si>
+  <si>
+    <t>C/ Neptuno</t>
+  </si>
+  <si>
+    <t>79503962T</t>
+  </si>
+  <si>
+    <t>Cristina</t>
+  </si>
+  <si>
+    <t>Lemke</t>
+  </si>
+  <si>
+    <t>Rutherford</t>
+  </si>
+  <si>
+    <t>C/ Saturno</t>
+  </si>
+  <si>
+    <t>82842571K</t>
+  </si>
+  <si>
+    <t>Ramón</t>
+  </si>
+  <si>
+    <t>Herzog</t>
+  </si>
+  <si>
+    <t>Tremblay</t>
+  </si>
+  <si>
+    <t>C/ Urano</t>
+  </si>
+  <si>
+    <t>61142000L</t>
+  </si>
+  <si>
+    <t>Esther</t>
+  </si>
+  <si>
+    <t>Spencer</t>
+  </si>
+  <si>
+    <t>Lakin</t>
+  </si>
+  <si>
+    <t>C/ Plutón</t>
+  </si>
+  <si>
+    <t>46900725E</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Herman</t>
+  </si>
+  <si>
+    <t>Pacocha</t>
+  </si>
+  <si>
+    <t>C/ Andarax</t>
+  </si>
+  <si>
+    <t>85366986W</t>
+  </si>
+  <si>
+    <t>Carmen</t>
+  </si>
+  <si>
+    <t>Streich</t>
+  </si>
+  <si>
+    <t>Hirthe</t>
+  </si>
+  <si>
+    <t>C/ Almanzora</t>
+  </si>
+  <si>
+    <t>73571384L</t>
+  </si>
+  <si>
+    <t>Alfredo</t>
+  </si>
+  <si>
+    <t>Stiedemann</t>
+  </si>
+  <si>
+    <t>Morissette</t>
+  </si>
+  <si>
+    <t>C/ Guadalquivir</t>
+  </si>
+  <si>
+    <t>82937751G</t>
+  </si>
+  <si>
+    <t>Manolo</t>
+  </si>
+  <si>
+    <t>Hamill</t>
+  </si>
+  <si>
+    <t>Kozey</t>
+  </si>
+  <si>
+    <t>C/ Duero</t>
+  </si>
+  <si>
+    <t>80502866Z</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>Kohler</t>
+  </si>
+  <si>
+    <t>Schoen</t>
+  </si>
+  <si>
+    <t>C/ Tajo</t>
+  </si>
+  <si>
+    <t>10485008K</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>Fahey</t>
+  </si>
+  <si>
+    <t>Considine</t>
+  </si>
+  <si>
+    <t>C/ Sierra de los Filabres</t>
+  </si>
+  <si>
+    <t>85869555K</t>
+  </si>
+  <si>
+    <t>Guillermo</t>
+  </si>
+  <si>
+    <t>Ruecker</t>
+  </si>
+  <si>
+    <t>Upton</t>
+  </si>
+  <si>
+    <t>C/ Sierra de Gádor</t>
+  </si>
+  <si>
+    <t>04326833G</t>
+  </si>
+  <si>
+    <t>Micaela</t>
+  </si>
+  <si>
+    <t>Monahan</t>
+  </si>
+  <si>
+    <t>Murray</t>
+  </si>
+  <si>
+    <t>C/ Veleta</t>
+  </si>
+  <si>
+    <t>11578526G</t>
+  </si>
+  <si>
+    <t>Inma</t>
+  </si>
+  <si>
+    <t>Yundt</t>
+  </si>
+  <si>
+    <t>C/ Picos de Europa</t>
+  </si>
+  <si>
+    <t>79221403L</t>
+  </si>
+  <si>
+    <t>Francesca</t>
+  </si>
+  <si>
+    <t>Schowalter</t>
+  </si>
+  <si>
+    <t>Muller</t>
+  </si>
+  <si>
+    <t>C/ Quinto pino</t>
+  </si>
+  <si>
+    <t>79089577Y</t>
+  </si>
+  <si>
+    <t>Gutiérrez</t>
+  </si>
+  <si>
+    <t>López</t>
+  </si>
+  <si>
+    <t>C/ Los pinos</t>
+  </si>
+  <si>
+    <t>41491230N</t>
+  </si>
+  <si>
+    <t>Domínguez</t>
+  </si>
+  <si>
+    <t>Guerrero</t>
+  </si>
+  <si>
+    <t>C/ Cabo de Gata</t>
+  </si>
+  <si>
+    <t>64753215G</t>
+  </si>
+  <si>
+    <t>Irene</t>
+  </si>
+  <si>
+    <t>Hernández</t>
+  </si>
+  <si>
+    <t>Martínez</t>
+  </si>
+  <si>
+    <t>C/ Zapillo</t>
+  </si>
+  <si>
+    <t>85135690V</t>
+  </si>
+  <si>
+    <t>Sonia</t>
+  </si>
+  <si>
+    <t>Ruiz</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>nif</t>
+  </si>
+  <si>
+    <t>apellido1</t>
+  </si>
+  <si>
+    <t>apellido2</t>
+  </si>
+  <si>
+    <t>ciudad</t>
+  </si>
+  <si>
+    <t>direccion</t>
+  </si>
+  <si>
+    <t>teléfono</t>
+  </si>
+  <si>
+    <t>fecha de nacimiento</t>
+  </si>
+  <si>
+    <t>sexo</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>id_profesor</t>
+  </si>
+  <si>
+    <t>id_departamento</t>
+  </si>
+  <si>
+    <t>Retorna un llistat amb els professors/es que no imparteixen cap assignatura.</t>
+  </si>
+  <si>
+    <t>Calcula quants/es professors/es hi ha en cada departament. 
+El resultat només ha de mostrar dues columnes, una amb el nom del departament i una altra amb el nombre de professors/es que hi ha en aquest departament. 
+El resultat només ha d'incloure els departaments que tenen professors/es associats i haurà d'estar ordenat de major a menor pel nombre de professors/es.</t>
+  </si>
+  <si>
+    <t>Devuelve un listado con todos los departamentos y el número de profesores/as que hay en cada uno de ellos.
+Tiene en cuenta que pueden existir departamentos que no tienen profesores/as asociados/as.
+Estos departamentos también deben aparecer en el listado.</t>
+  </si>
+  <si>
+    <t>Retorna un llistat amb el nom de tots els graus existents en la base de dades i el nombre d'assignatures que té cadascun, dels graus que tinguin més de 40 assignatures associades.</t>
+  </si>
+  <si>
+    <t>Devuelve un listado con el nombre de todos los grados existentes en la base de datos y el número de asignaturas que tiene cada uno. 
+Tiene en cuenta que pueden existir grados que carecen de asignaturas asociadas. 
+Estos grados también deben aparecer en el listado. 
+El resultado deberá estar ordenado de mayor a menor por el número de asignaturas</t>
   </si>
 </sst>
 </file>
@@ -393,7 +801,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,6 +823,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -490,6 +904,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1202,26 +1625,1056 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5DD659F-EA35-467C-B419-FF376CE605B4}">
-  <dimension ref="A1"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="6">
+        <v>950254837</v>
+      </c>
+      <c r="I2" s="20">
+        <v>33325</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="6">
+        <v>618253876</v>
+      </c>
+      <c r="I3" s="20">
+        <v>33824</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="6">
+        <v>618223876</v>
+      </c>
+      <c r="I4" s="20">
+        <v>29086</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L4" t="e">
+        <f>VLOOKUP(A4,profesor!$A$2:$A$12,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="20">
+        <v>36804</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="6">
+        <v>678516294</v>
+      </c>
+      <c r="I6" s="20">
+        <v>28509</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L6">
+        <f>VLOOKUP(A6,profesor!$A$2:$A$12,1,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" s="6">
+        <v>628349590</v>
+      </c>
+      <c r="I7" s="20">
+        <v>35823</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="20">
+        <v>36304</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" s="6">
+        <v>669162534</v>
+      </c>
+      <c r="I9" s="20">
+        <v>28358</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L9">
+        <f>VLOOKUP(A9,profesor!$A$2:$A$12,1,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H10" s="6">
+        <v>626351429</v>
+      </c>
+      <c r="I10" s="20">
+        <v>35390</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="20">
+        <v>28264</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L11">
+        <f>VLOOKUP(A11,profesor!$A$2:$A$12,1,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="H12" s="6">
+        <v>679837625</v>
+      </c>
+      <c r="I12" s="20">
+        <v>35546</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="20">
+        <v>26052</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L13">
+        <f>VLOOKUP(A13,profesor!$A$2:$A$12,1,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="H14" s="6">
+        <v>950896725</v>
+      </c>
+      <c r="I14" s="20">
+        <v>29252</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L14">
+        <f>VLOOKUP(A14,profesor!$A$2:$A$12,1,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="H15" s="6">
+        <v>950263514</v>
+      </c>
+      <c r="I15" s="20">
+        <v>28127</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L15">
+        <f>VLOOKUP(A15,profesor!$A$2:$A$12,1,0)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="H16" s="6">
+        <v>668726354</v>
+      </c>
+      <c r="I16" s="20">
+        <v>29294</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L16">
+        <f>VLOOKUP(A16,profesor!$A$2:$A$12,1,0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="20">
+        <v>30028</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L17">
+        <f>VLOOKUP(A17,profesor!$A$2:$A$12,1,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="20">
+        <v>26789</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L18">
+        <f>VLOOKUP(A18,profesor!$A$2:$A$12,1,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="H19" s="6">
+        <v>662765413</v>
+      </c>
+      <c r="I19" s="20">
+        <v>27815</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L19">
+        <f>VLOOKUP(A19,profesor!$A$2:$A$12,1,0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H20" s="6">
+        <v>678652431</v>
+      </c>
+      <c r="I20" s="20">
+        <v>36039</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="20">
+        <v>29525</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L21">
+        <f>VLOOKUP(A21,profesor!$A$2:$A$12,1,0)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H22" s="6">
+        <v>678652431</v>
+      </c>
+      <c r="I22" s="20">
+        <v>35796</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H23" s="6">
+        <v>626652498</v>
+      </c>
+      <c r="I23" s="20">
+        <v>36202</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H24" s="6">
+        <v>628452384</v>
+      </c>
+      <c r="I24" s="20">
+        <v>35136</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H25" s="6">
+        <v>678812017</v>
+      </c>
+      <c r="I25" s="20">
+        <v>34802</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:K25" xr:uid="{E5DD659F-EA35-467C-B419-FF376CE605B4}">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="profesor"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C19AC5-F112-4205-A84D-1D30622B7634}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>5</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>15</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>12</v>
+      </c>
+      <c r="B8" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="6">
+        <v>20</v>
+      </c>
+      <c r="B12" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{75C19AC5-F112-4205-A84D-1D30622B7634}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1523,14 +2976,14 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:B10"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.1796875" style="15" customWidth="1"/>
-    <col min="2" max="2" width="104.7265625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="145.54296875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -1555,7 +3008,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -1592,7 +3045,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31" x14ac:dyDescent="0.35">
@@ -1601,7 +3054,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31" x14ac:dyDescent="0.35">
@@ -1610,15 +3063,15 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31" x14ac:dyDescent="0.35">
-      <c r="A10" s="15">
+      <c r="A10" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="5" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1627,115 +3080,115 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="62" x14ac:dyDescent="0.35">
-      <c r="A12" s="15">
+    <row r="12" spans="1:3" ht="93" x14ac:dyDescent="0.35">
+      <c r="A12" s="18">
         <v>1</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>77</v>
+      <c r="B12" s="19" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="15">
+      <c r="A13" s="18">
         <f>A12+1</f>
         <v>2</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>78</v>
+      <c r="B13" s="19" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="15">
+      <c r="A14" s="17">
         <f t="shared" ref="A14:A17" si="1">A13+1</f>
         <v>3</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>79</v>
+      <c r="B14" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="15">
+      <c r="A15" s="17">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>80</v>
+      <c r="B15" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="15">
+      <c r="A16" s="17">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>81</v>
+      <c r="B16" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="15">
+      <c r="A17" s="17">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>82</v>
+      <c r="B17" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B18" s="16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="15">
+      <c r="A19" s="17">
         <v>1</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>84</v>
+      <c r="B19" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="15">
+      <c r="A20" s="17">
         <f>A19+1</f>
         <v>2</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>85</v>
+      <c r="B20" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="62" x14ac:dyDescent="0.35">
-      <c r="A21" s="15">
+      <c r="A21" s="17">
         <f t="shared" ref="A21:A29" si="2">A20+1</f>
         <v>3</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>86</v>
+      <c r="B21" s="5" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="15">
+      <c r="A22" s="17">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="15">
+      <c r="B22" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+      <c r="A23" s="17">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>88</v>
+      <c r="B23" s="5" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A24" s="15">
+      <c r="A24" s="18">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>89</v>
+      <c r="B24" s="19" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
@@ -1744,7 +3197,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
@@ -1753,7 +3206,7 @@
         <v>8</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="62" x14ac:dyDescent="0.35">
@@ -1762,7 +3215,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -1771,7 +3224,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="31" x14ac:dyDescent="0.35">
@@ -1780,7 +3233,7 @@
         <v>11</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Universidad excercise done, two missing
</commit_message>
<xml_diff>
--- a/Sprint2Tema1Ejercicios.xlsx
+++ b/Sprint2Tema1Ejercicios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Barajas\Desktop\02 PHP FULL STACK\Sprint 2\Sprint2Tema1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD5404C-4815-49D0-BF02-C967619AA520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B0C7BB-5CCD-4B2C-8D56-5C9C438BB0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="466" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -302,21 +302,6 @@
     <t>2. Calcula quants/es alumnes van néixer en 1999.</t>
   </si>
   <si>
-    <t>7. Retorna un llistat que mostri el nom dels graus i la suma del nombre total de crèdits que hi ha per a cada tipus d'assignatura. El resultat ha de tenir tres columnes: nom del grau, tipus d'assignatura i la suma dels crèdits de totes les assignatures que hi ha d'aquest tipus.</t>
-  </si>
-  <si>
-    <t>8. Retorna un llistat que mostri quants/es alumnes s'han matriculat d'alguna assignatura en cadascun dels cursos escolars. El resultat haurà de mostrar dues columnes, una columna amb l'any d'inici del curs escolar i una altra amb el nombre d'alumnes matriculats/des.</t>
-  </si>
-  <si>
-    <t>9. Retorna un llistat amb el nombre d'assignatures que imparteix cada professor/a. El llistat ha de tenir en compte aquells professors/es que no imparteixen cap assignatura. El resultat mostrarà cinc columnes: id, nom, primer cognom, segon cognom i nombre d'assignatures. El resultat estarà ordenat de major a menor pel nombre d'assignatures.</t>
-  </si>
-  <si>
-    <t>10. Retorna totes les dades de l'alumne més jove.</t>
-  </si>
-  <si>
-    <t>11. Retorna un llistat amb els professors/es que tenen un departament associat i que no imparteixen cap assignatura.</t>
-  </si>
-  <si>
     <t>Halla el nombre y los dos apellidos de los alumnos que no han dado de alta su número de teléfono en la base de datos.</t>
   </si>
   <si>
@@ -756,6 +741,25 @@
 Tiene en cuenta que pueden existir grados que carecen de asignaturas asociadas. 
 Estos grados también deben aparecer en el listado. 
 El resultado deberá estar ordenado de mayor a menor por el número de asignaturas</t>
+  </si>
+  <si>
+    <t>Devuelve un listado que muestre el nombre de los grados y 
+la suma del número total de créditos existentes para cada tipo de asignatura. 
+El resultado debe tener tres columnas: nombre del grado, tipo de asignatura y la suma de los créditos de todas las asignaturas que existen de este tipo.</t>
+  </si>
+  <si>
+    <t>Devuelve un listado con el número de asignaturas que imparte cada profesor/a. El listado debe tener en cuenta a aquellos profesores/as que no imparten ninguna asignatura. El resultado mostrará cinco columnas: id, nombre, primer apellido, segundo apellido y número de asignaturas. El resultado estará ordenado de mayor a menor por el número de asignaturas.</t>
+  </si>
+  <si>
+    <t>Devuelve un listado que muestre cuántos/as alumnos/as se han matriculado de alguna asignatura en cada uno de los cursos escolares. 
+El resultado deberá mostrar dos columnas, una columna con el año de inicio del curso escolar 
+y otra con el número de alumnos/as matriculados/as.</t>
+  </si>
+  <si>
+    <t>Retorna totes les dades de l'alumne més jove.</t>
+  </si>
+  <si>
+    <t>Retorna un llistat amb els professors/es que tenen un departament associat i que no imparteixen cap assignatura.</t>
   </si>
 </sst>
 </file>
@@ -1639,37 +1643,37 @@
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>218</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1677,22 +1681,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="H2" s="6">
         <v>950254837</v>
@@ -1701,10 +1705,10 @@
         <v>33325</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
@@ -1712,22 +1716,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H3" s="6">
         <v>618253876</v>
@@ -1736,10 +1740,10 @@
         <v>33824</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -1747,22 +1751,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H4" s="6">
         <v>618223876</v>
@@ -1771,10 +1775,10 @@
         <v>29086</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L4" t="e">
         <f>VLOOKUP(A4,profesor!$A$2:$A$12,1,0)</f>
@@ -1786,32 +1790,32 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="20">
         <v>36804</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -1819,22 +1823,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H6" s="6">
         <v>678516294</v>
@@ -1843,10 +1847,10 @@
         <v>28509</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L6">
         <f>VLOOKUP(A6,profesor!$A$2:$A$12,1,0)</f>
@@ -1858,22 +1862,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H7" s="6">
         <v>628349590</v>
@@ -1882,10 +1886,10 @@
         <v>35823</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
@@ -1893,32 +1897,32 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="20">
         <v>36304</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -1926,22 +1930,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H9" s="6">
         <v>669162534</v>
@@ -1950,10 +1954,10 @@
         <v>28358</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L9">
         <f>VLOOKUP(A9,profesor!$A$2:$A$12,1,0)</f>
@@ -1965,22 +1969,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H10" s="6">
         <v>626351429</v>
@@ -1989,10 +1993,10 @@
         <v>35390</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -2000,32 +2004,32 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="20">
         <v>28264</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L11">
         <f>VLOOKUP(A11,profesor!$A$2:$A$12,1,0)</f>
@@ -2037,22 +2041,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H12" s="6">
         <v>679837625</v>
@@ -2061,10 +2065,10 @@
         <v>35546</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2072,32 +2076,32 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="20">
         <v>26052</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L13">
         <f>VLOOKUP(A13,profesor!$A$2:$A$12,1,0)</f>
@@ -2109,22 +2113,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H14" s="6">
         <v>950896725</v>
@@ -2133,10 +2137,10 @@
         <v>29252</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L14">
         <f>VLOOKUP(A14,profesor!$A$2:$A$12,1,0)</f>
@@ -2148,22 +2152,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H15" s="6">
         <v>950263514</v>
@@ -2172,10 +2176,10 @@
         <v>28127</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L15">
         <f>VLOOKUP(A15,profesor!$A$2:$A$12,1,0)</f>
@@ -2187,22 +2191,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H16" s="6">
         <v>668726354</v>
@@ -2211,10 +2215,10 @@
         <v>29294</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L16">
         <f>VLOOKUP(A16,profesor!$A$2:$A$12,1,0)</f>
@@ -2226,32 +2230,32 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="20">
         <v>30028</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L17">
         <f>VLOOKUP(A17,profesor!$A$2:$A$12,1,0)</f>
@@ -2263,32 +2267,32 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="20">
         <v>26789</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L18">
         <f>VLOOKUP(A18,profesor!$A$2:$A$12,1,0)</f>
@@ -2300,22 +2304,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H19" s="6">
         <v>662765413</v>
@@ -2324,10 +2328,10 @@
         <v>27815</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L19">
         <f>VLOOKUP(A19,profesor!$A$2:$A$12,1,0)</f>
@@ -2339,22 +2343,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H20" s="6">
         <v>678652431</v>
@@ -2363,10 +2367,10 @@
         <v>36039</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2374,32 +2378,32 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="20">
         <v>29525</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L21">
         <f>VLOOKUP(A21,profesor!$A$2:$A$12,1,0)</f>
@@ -2411,22 +2415,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H22" s="6">
         <v>678652431</v>
@@ -2435,10 +2439,10 @@
         <v>35796</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2446,22 +2450,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H23" s="6">
         <v>626652498</v>
@@ -2470,10 +2474,10 @@
         <v>36202</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
@@ -2481,22 +2485,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H24" s="6">
         <v>628452384</v>
@@ -2505,10 +2509,10 @@
         <v>35136</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
@@ -2516,22 +2520,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H25" s="6">
         <v>678812017</v>
@@ -2540,10 +2544,10 @@
         <v>34802</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2575,10 +2579,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2976,8 +2980,8 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3002,13 +3006,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="17">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -3021,7 +3025,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3030,7 +3034,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="17">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3045,7 +3049,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31" x14ac:dyDescent="0.35">
@@ -3054,7 +3058,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31" x14ac:dyDescent="0.35">
@@ -3063,7 +3067,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31" x14ac:dyDescent="0.35">
@@ -3080,12 +3084,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="93" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="62" x14ac:dyDescent="0.35">
       <c r="A12" s="18">
         <v>1</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -3094,7 +3098,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -3112,7 +3116,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -3161,7 +3165,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
@@ -3170,7 +3174,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="62" x14ac:dyDescent="0.35">
@@ -3179,7 +3183,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="31" x14ac:dyDescent="0.35">
@@ -3188,52 +3192,52 @@
         <v>6</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="15">
+      <c r="A25" s="17">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>83</v>
+      <c r="B25" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="15">
+      <c r="A26" s="18">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="62" x14ac:dyDescent="0.35">
-      <c r="A27" s="15">
+      <c r="B26" s="19" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="18">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>85</v>
+      <c r="B27" s="19" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="15">
+      <c r="A28" s="18">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="B28" s="19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>87</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>